<commit_message>
Added an option for top 100 by adult mean word count
</commit_message>
<xml_diff>
--- a/output/SAMPLE_INPUT_50snippets_random.xlsx
+++ b/output/SAMPLE_INPUT_50snippets_random.xlsx
@@ -472,121 +472,121 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5:45 AM</t>
+          <t>5:37 AM</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1169.48</v>
+        <v>729.045</v>
       </c>
       <c r="D2" t="n">
-        <v>1199.48</v>
+        <v>759.045</v>
       </c>
       <c r="E2" t="n">
-        <v>21.87</v>
+        <v>11.335</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5:50 AM</t>
+          <t>5:58 AM</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1489.303333</v>
+        <v>1964.125</v>
       </c>
       <c r="D3" t="n">
-        <v>1519.303333</v>
+        <v>1994.125</v>
       </c>
       <c r="E3" t="n">
-        <v>2.51</v>
+        <v>1.13</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>6:07 AM</t>
+          <t>6:09 AM</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2509.07</v>
+        <v>2629.6425</v>
       </c>
       <c r="D4" t="n">
-        <v>2539.07</v>
+        <v>2659.6425</v>
       </c>
       <c r="E4" t="n">
-        <v>3.404</v>
+        <v>5.215</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>6:11 AM</t>
+          <t>6:13 AM</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2774.6</v>
+        <v>2882.4</v>
       </c>
       <c r="D5" t="n">
-        <v>2804.6</v>
+        <v>2912.4</v>
       </c>
       <c r="E5" t="n">
-        <v>16.77</v>
+        <v>19.2</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6:16 AM</t>
+          <t>6:27 AM</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3079.71</v>
+        <v>3732.76</v>
       </c>
       <c r="D6" t="n">
-        <v>3109.71</v>
+        <v>3762.76</v>
       </c>
       <c r="E6" t="n">
-        <v>14.55</v>
+        <v>14.64</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -597,71 +597,71 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6:23 AM</t>
+          <t>6:34 AM</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3473.17</v>
+        <v>4149.392</v>
       </c>
       <c r="D7" t="n">
-        <v>3503.17</v>
+        <v>4179.392</v>
       </c>
       <c r="E7" t="n">
-        <v>1.063333</v>
+        <v>1.24</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.333333</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6:34 AM</t>
+          <t>6:41 AM</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4149.392</v>
+        <v>4544.685</v>
       </c>
       <c r="D8" t="n">
-        <v>4179.392</v>
+        <v>4574.685</v>
       </c>
       <c r="E8" t="n">
-        <v>1.24</v>
+        <v>4.463333</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2</v>
+        <v>0.166667</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>6:38 AM</t>
+          <t>6:45 AM</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4379.04</v>
+        <v>4808.78</v>
       </c>
       <c r="D9" t="n">
-        <v>4409.04</v>
+        <v>4838.78</v>
       </c>
       <c r="E9" t="n">
-        <v>3.49</v>
+        <v>2.95</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -672,21 +672,21 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6:50 AM</t>
+          <t>6:52 AM</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>5077.825</v>
+        <v>5193.04</v>
       </c>
       <c r="D10" t="n">
-        <v>5107.825</v>
+        <v>5223.04</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4025</v>
+        <v>71.97</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -697,21 +697,21 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>6:54 AM</t>
+          <t>6:56 AM</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>5358.123333</v>
+        <v>5440.89</v>
       </c>
       <c r="D11" t="n">
-        <v>5388.123333</v>
+        <v>5470.89</v>
       </c>
       <c r="E11" t="n">
-        <v>1.47</v>
+        <v>108.74</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -722,46 +722,46 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>198</v>
+        <v>236</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7:04 AM</t>
+          <t>7:23 AM</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>5933.15</v>
+        <v>7065.746667</v>
       </c>
       <c r="D12" t="n">
-        <v>5963.15</v>
+        <v>7095.746667</v>
       </c>
       <c r="E12" t="n">
-        <v>1.195</v>
+        <v>0.863333</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.5</v>
+        <v>0.333333</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>214</v>
+        <v>248</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>7:12 AM</t>
+          <t>7:29 AM</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>6404.45</v>
+        <v>7417.6925</v>
       </c>
       <c r="D13" t="n">
-        <v>6434.45</v>
+        <v>7447.6925</v>
       </c>
       <c r="E13" t="n">
-        <v>1.525</v>
+        <v>3.91</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -772,46 +772,46 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>221</v>
+        <v>256</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>7:16 AM</t>
+          <t>7:33 AM</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6626.76</v>
+        <v>7665.623333</v>
       </c>
       <c r="D14" t="n">
-        <v>6656.76</v>
+        <v>7695.623333</v>
       </c>
       <c r="E14" t="n">
-        <v>3.56</v>
+        <v>5.7</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>0.346667</v>
       </c>
       <c r="G14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>250</v>
+        <v>290</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>7:30 AM</t>
+          <t>7:50 AM</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>7488.7825</v>
+        <v>8698.795</v>
       </c>
       <c r="D15" t="n">
-        <v>7518.7825</v>
+        <v>8728.795</v>
       </c>
       <c r="E15" t="n">
-        <v>0.08749999999999999</v>
+        <v>1.96</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -822,46 +822,46 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>277</v>
+        <v>303</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>7:43 AM</t>
+          <t>7:56 AM</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>8299.91</v>
+        <v>9072.33</v>
       </c>
       <c r="D16" t="n">
-        <v>8329.91</v>
+        <v>9102.33</v>
       </c>
       <c r="E16" t="n">
-        <v>4.62</v>
+        <v>3.06</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>8:16 AM</t>
+          <t>8:19 AM</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>10238.38</v>
+        <v>10459.5</v>
       </c>
       <c r="D17" t="n">
-        <v>10268.38</v>
+        <v>10489.5</v>
       </c>
       <c r="E17" t="n">
-        <v>2.085</v>
+        <v>1.52</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -872,49 +872,49 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>387</v>
+        <v>362</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>8:39 AM</t>
+          <t>8:26 AM</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>11609.42</v>
+        <v>10841.275</v>
       </c>
       <c r="D18" t="n">
-        <v>11639.42</v>
+        <v>10871.275</v>
       </c>
       <c r="E18" t="n">
-        <v>8.06</v>
+        <v>4.755</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>425</v>
+        <v>372</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>8:57 AM</t>
+          <t>8:31 AM</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>12725.265</v>
+        <v>11144.155</v>
       </c>
       <c r="D19" t="n">
-        <v>12755.265</v>
+        <v>11174.155</v>
       </c>
       <c r="E19" t="n">
-        <v>4.76</v>
+        <v>5.175</v>
       </c>
       <c r="F19" t="n">
-        <v>43.895</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
@@ -922,121 +922,121 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>435</v>
+        <v>381</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>9:02 AM</t>
+          <t>8:35 AM</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>13043.06</v>
+        <v>11413.92</v>
       </c>
       <c r="D20" t="n">
-        <v>13073.06</v>
+        <v>11443.92</v>
       </c>
       <c r="E20" t="n">
-        <v>4.12</v>
+        <v>1.94</v>
       </c>
       <c r="F20" t="n">
-        <v>1.68</v>
+        <v>19.395</v>
       </c>
       <c r="G20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>443</v>
+        <v>398</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>9:06 AM</t>
+          <t>8:44 AM</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>13276.226667</v>
+        <v>11919.3225</v>
       </c>
       <c r="D21" t="n">
-        <v>13306.226667</v>
+        <v>11949.3225</v>
       </c>
       <c r="E21" t="n">
-        <v>1.58</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
-        <v>5.873333</v>
+        <v>2.18</v>
       </c>
       <c r="G21" t="n">
-        <v>0.333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>451</v>
+        <v>515</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>9:10 AM</t>
+          <t>9:43 AM</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>13511.86</v>
+        <v>15448.26</v>
       </c>
       <c r="D22" t="n">
-        <v>13541.86</v>
+        <v>15478.26</v>
       </c>
       <c r="E22" t="n">
-        <v>5.205</v>
+        <v>2.15</v>
       </c>
       <c r="F22" t="n">
-        <v>10.74</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>9:58 AM</t>
+          <t>10:00 A</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>16367.32</v>
+        <v>16484</v>
       </c>
       <c r="D23" t="n">
-        <v>16397.32</v>
+        <v>16514</v>
       </c>
       <c r="E23" t="n">
-        <v>2.1925</v>
+        <v>26.08</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>567</v>
+        <v>980</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>10:08 A</t>
+          <t>1:35 PM</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>16994.61</v>
+        <v>29392.66</v>
       </c>
       <c r="D24" t="n">
-        <v>17024.61</v>
+        <v>29422.66</v>
       </c>
       <c r="E24" t="n">
-        <v>7.28</v>
+        <v>6.8</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -1047,21 +1047,21 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>575</v>
+        <v>987</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>10:12 A</t>
+          <t>1:39 PM</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>17229.33</v>
+        <v>29607.37</v>
       </c>
       <c r="D25" t="n">
-        <v>17259.33</v>
+        <v>29637.37</v>
       </c>
       <c r="E25" t="n">
-        <v>1.03</v>
+        <v>3.695</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -1072,99 +1072,99 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>981</v>
+        <v>998</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1:35 PM</t>
+          <t>1:44 PM</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>29415.15</v>
+        <v>29923.235</v>
       </c>
       <c r="D26" t="n">
-        <v>29445.15</v>
+        <v>29953.235</v>
       </c>
       <c r="E26" t="n">
-        <v>13.746667</v>
+        <v>7.655</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>990</v>
+        <v>1034</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1:40 PM</t>
+          <t>2:02 PM</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>29686.38</v>
+        <v>31003.725</v>
       </c>
       <c r="D27" t="n">
-        <v>29716.38</v>
+        <v>31033.725</v>
       </c>
       <c r="E27" t="n">
-        <v>5.98</v>
+        <v>8.225</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1012</v>
+        <v>1054</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1:51 PM</t>
+          <t>2:12 PM</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>30341.53</v>
+        <v>31608.545</v>
       </c>
       <c r="D28" t="n">
-        <v>30371.53</v>
+        <v>31638.545</v>
       </c>
       <c r="E28" t="n">
-        <v>6.06</v>
+        <v>1.995</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1035</v>
+        <v>1064</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2:02 PM</t>
+          <t>2:17 PM</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>31029.245</v>
+        <v>31902.553333</v>
       </c>
       <c r="D29" t="n">
-        <v>31059.245</v>
+        <v>31932.553333</v>
       </c>
       <c r="E29" t="n">
-        <v>17.475</v>
+        <v>10.7</v>
       </c>
       <c r="F29" t="n">
-        <v>0.545</v>
+        <v>0</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
@@ -1172,21 +1172,21 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1048</v>
+        <v>1085</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2:09 PM</t>
+          <t>2:27 PM</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>31421.85</v>
+        <v>32536.5</v>
       </c>
       <c r="D30" t="n">
-        <v>31451.85</v>
+        <v>32566.5</v>
       </c>
       <c r="E30" t="n">
-        <v>4.695</v>
+        <v>0.8375</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -1197,71 +1197,71 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1104</v>
+        <v>1092</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2:37 PM</t>
+          <t>2:31 PM</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>33100.574</v>
+        <v>32747.78</v>
       </c>
       <c r="D31" t="n">
-        <v>33130.574</v>
+        <v>32777.78</v>
       </c>
       <c r="E31" t="n">
-        <v>2.998</v>
+        <v>1.665</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1141</v>
+        <v>1103</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2:55 PM</t>
+          <t>2:36 PM</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>34219.87</v>
+        <v>33070.88</v>
       </c>
       <c r="D32" t="n">
-        <v>34249.87</v>
+        <v>33100.88</v>
       </c>
       <c r="E32" t="n">
-        <v>21.48</v>
+        <v>25.1</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1157</v>
+        <v>1172</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>3:03 PM</t>
+          <t>3:11 PM</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>34686.29</v>
+        <v>35139.775</v>
       </c>
       <c r="D33" t="n">
-        <v>34716.29</v>
+        <v>35169.775</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>14.545</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -1272,21 +1272,21 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1192</v>
+        <v>1195</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3:21 PM</t>
+          <t>3:22 PM</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>35742.3425</v>
+        <v>35827.2775</v>
       </c>
       <c r="D34" t="n">
-        <v>35772.3425</v>
+        <v>35857.2775</v>
       </c>
       <c r="E34" t="n">
-        <v>13.795</v>
+        <v>4.8075</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -1297,46 +1297,46 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1214</v>
+        <v>1243</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3:32 PM</t>
+          <t>3:46 PM</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>36391.61</v>
+        <v>37267.225</v>
       </c>
       <c r="D35" t="n">
-        <v>36421.61</v>
+        <v>37297.225</v>
       </c>
       <c r="E35" t="n">
-        <v>96.52</v>
+        <v>9.237500000000001</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1224</v>
+        <v>1254</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>3:37 PM</t>
+          <t>3:52 PM</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>36710.185</v>
+        <v>37603.08</v>
       </c>
       <c r="D36" t="n">
-        <v>36740.185</v>
+        <v>37633.08</v>
       </c>
       <c r="E36" t="n">
-        <v>3.49</v>
+        <v>3.615</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -1347,21 +1347,21 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1242</v>
+        <v>1263</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>3:46 PM</t>
+          <t>3:57 PM</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>37247.11</v>
+        <v>37889.45</v>
       </c>
       <c r="D37" t="n">
-        <v>37277.11</v>
+        <v>37919.45</v>
       </c>
       <c r="E37" t="n">
-        <v>5.1975</v>
+        <v>3.78</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
@@ -1372,46 +1372,46 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1257</v>
+        <v>1271</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3:53 PM</t>
+          <t>4:00 PM</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>37684.8</v>
+        <v>38112.49</v>
       </c>
       <c r="D38" t="n">
-        <v>37714.8</v>
+        <v>38142.49</v>
       </c>
       <c r="E38" t="n">
-        <v>36.82</v>
+        <v>8.436667</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1267</v>
+        <v>1297</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>3:58 PM</t>
+          <t>4:13 PM</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>37993.783333</v>
+        <v>38885.46</v>
       </c>
       <c r="D39" t="n">
-        <v>38023.783333</v>
+        <v>38915.46</v>
       </c>
       <c r="E39" t="n">
-        <v>5.263333</v>
+        <v>73.44</v>
       </c>
       <c r="F39" t="n">
         <v>0</v>
@@ -1422,21 +1422,21 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1279</v>
+        <v>1308</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4:05 PM</t>
+          <t>4:19 PM</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>38365.04</v>
+        <v>39217.913333</v>
       </c>
       <c r="D40" t="n">
-        <v>38395.04</v>
+        <v>39247.913333</v>
       </c>
       <c r="E40" t="n">
-        <v>31.16</v>
+        <v>29.03</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -1447,277 +1447,277 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1295</v>
+        <v>1335</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4:12 PM</t>
+          <t>4:32 PM</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>38838.2425</v>
+        <v>40027.72</v>
       </c>
       <c r="D41" t="n">
-        <v>38868.2425</v>
+        <v>40057.72</v>
       </c>
       <c r="E41" t="n">
-        <v>18.295</v>
+        <v>47.705</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1328</v>
+        <v>1360</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4:29 PM</t>
+          <t>4:45 PM</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>39833.97</v>
+        <v>40775.5</v>
       </c>
       <c r="D42" t="n">
-        <v>39863.97</v>
+        <v>40805.5</v>
       </c>
       <c r="E42" t="n">
-        <v>12.77</v>
+        <v>27.96</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1338</v>
+        <v>1370</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4:34 PM</t>
+          <t>4:50 PM</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>40124.17</v>
+        <v>41074.77</v>
       </c>
       <c r="D43" t="n">
-        <v>40154.17</v>
+        <v>41104.77</v>
       </c>
       <c r="E43" t="n">
-        <v>10.0375</v>
+        <v>24.045</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1353</v>
+        <v>1393</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4:42 PM</t>
+          <t>5:01 PM</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>40589.99</v>
+        <v>41774.303333</v>
       </c>
       <c r="D44" t="n">
-        <v>40619.99</v>
+        <v>41804.303333</v>
       </c>
       <c r="E44" t="n">
-        <v>4.08</v>
+        <v>14.303333</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>0.333333</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1361</v>
+        <v>1401</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>4:45 PM</t>
+          <t>5:06 PM</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>40805.985</v>
+        <v>42025.86</v>
       </c>
       <c r="D45" t="n">
-        <v>40835.985</v>
+        <v>42055.86</v>
       </c>
       <c r="E45" t="n">
-        <v>17.225</v>
+        <v>3.2</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1370</v>
+        <v>1416</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>4:50 PM</t>
+          <t>5:13 PM</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>41074.77</v>
+        <v>42467.672</v>
       </c>
       <c r="D46" t="n">
-        <v>41104.77</v>
+        <v>42497.672</v>
       </c>
       <c r="E46" t="n">
-        <v>24.045</v>
+        <v>1.524</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1390</v>
+        <v>1432</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>5:21 PM</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>41680.48</v>
+        <v>42943.82</v>
       </c>
       <c r="D47" t="n">
-        <v>41710.48</v>
+        <v>42973.82</v>
       </c>
       <c r="E47" t="n">
-        <v>38.76</v>
+        <v>31.495</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1409</v>
+        <v>1445</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5:09 PM</t>
+          <t>5:27 PM</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>42250.0775</v>
+        <v>43323.345</v>
       </c>
       <c r="D48" t="n">
-        <v>42280.0775</v>
+        <v>43353.345</v>
       </c>
       <c r="E48" t="n">
-        <v>4.4525</v>
+        <v>29.31</v>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
+        <v>0.505</v>
       </c>
       <c r="G48" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1446</v>
+        <v>1482</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5:28 PM</t>
+          <t>5:46 PM</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>43374.21</v>
+        <v>44444.21</v>
       </c>
       <c r="D49" t="n">
-        <v>43404.21</v>
+        <v>44474.21</v>
       </c>
       <c r="E49" t="n">
-        <v>2.61</v>
+        <v>10.0225</v>
       </c>
       <c r="F49" t="n">
-        <v>0</v>
+        <v>0.5024999999999999</v>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1475</v>
+        <v>1534</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5:42 PM</t>
+          <t>6:12 PM</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>44227.06</v>
+        <v>46012.16</v>
       </c>
       <c r="D50" t="n">
-        <v>44257.06</v>
+        <v>46042.16</v>
       </c>
       <c r="E50" t="n">
-        <v>46.02</v>
+        <v>2.17</v>
       </c>
       <c r="F50" t="n">
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>1.333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1535</v>
+        <v>1546</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6:12 PM</t>
+          <t>6:18 PM</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>46024.31</v>
+        <v>46356.505</v>
       </c>
       <c r="D51" t="n">
-        <v>46054.31</v>
+        <v>46386.505</v>
       </c>
       <c r="E51" t="n">
-        <v>7.985</v>
+        <v>25.355</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>